<commit_message>
implement student choice parser for new domain
</commit_message>
<xml_diff>
--- a/hneu-personal-account-webapp/src/test/resources/parser/students_choice.xlsx
+++ b/hneu-personal-account-webapp/src/test/resources/parser/students_choice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oleksandrrozdolskyi/Repos/hneu-personal-account/src/test/resources/parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oleksandrrozdolskyi/Repos/hneu-personal-account/hneu-personal-account-webapp/src/test/resources/parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t xml:space="preserve">Прізвище </t>
   </si>
@@ -83,9 +83,6 @@
     <t>Семестр</t>
   </si>
   <si>
-    <t>Маг-майнер</t>
-  </si>
-  <si>
     <t>Назва</t>
   </si>
   <si>
@@ -96,13 +93,22 @@
   </si>
   <si>
     <t>Планування розвитку територій</t>
+  </si>
+  <si>
+    <t>Тип</t>
+  </si>
+  <si>
+    <t>МАЙНОР3</t>
+  </si>
+  <si>
+    <t>МАЙНОР1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +154,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,10 +246,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
@@ -542,7 +552,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,6 +563,7 @@
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="8.5" customWidth="1"/>
     <col min="6" max="6" width="56.5" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -572,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>16</v>
@@ -581,7 +592,7 @@
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -600,8 +611,8 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>22</v>
+      <c r="F2" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="G2" s="6">
         <v>1</v>
@@ -609,8 +620,8 @@
       <c r="H2" s="6">
         <v>1</v>
       </c>
-      <c r="I2" s="7">
-        <v>1</v>
+      <c r="I2" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -629,8 +640,8 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>21</v>
+      <c r="F3" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
@@ -638,11 +649,11 @@
       <c r="H3" s="6">
         <v>1</v>
       </c>
-      <c r="I3" s="7">
-        <v>2</v>
+      <c r="I3" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -658,8 +669,8 @@
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>20</v>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="G4" s="6">
         <v>1</v>
@@ -667,11 +678,11 @@
       <c r="H4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="7">
-        <v>1</v>
+      <c r="I4" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -687,8 +698,8 @@
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>21</v>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
@@ -696,8 +707,8 @@
       <c r="H5" s="6">
         <v>1</v>
       </c>
-      <c r="I5" s="7">
-        <v>2</v>
+      <c r="I5" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>